<commit_message>
push clean data of population_age_sex_race.csv and state_name_clean at resources
</commit_message>
<xml_diff>
--- a/Resources/kosal/SQL.xlsx
+++ b/Resources/kosal/SQL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science\Project2\senate-analysis\Resources\kosal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science\gitlab\project2\Finalwork\senate-analysis\resources\kosal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9FE391-06D1-4443-9EB4-F2BA1F3434A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FBC666-F3A1-452D-820B-1157CF0502FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12096" yWindow="12960" windowWidth="20640" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3468" yWindow="13560" windowWidth="20640" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>SEX</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>two+</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>87+</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>lost</t>
   </si>
 </sst>
 </file>
@@ -597,7 +609,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:F35"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,6 +743,23 @@
       </c>
       <c r="E11" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>